<commit_message>
fix display issues, add ball trials
</commit_message>
<xml_diff>
--- a/res/trials.xlsx
+++ b/res/trials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rima-mariarahal/science/globalbluegreen/globalbluegreen/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rima-mariarahal/science/nogago/nogago/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CA84EC-79F0-0446-B815-181A319A4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD1C0F4-6D26-C141-BF35-49CC98A8945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="2340" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{46A3392B-8735-774F-B60D-1E4EA857EEDA}"/>
+    <workbookView xWindow="2920" yWindow="-18560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{46A3392B-8735-774F-B60D-1E4EA857EEDA}"/>
   </bookViews>
   <sheets>
     <sheet name="prep" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>s1</t>
   </si>
@@ -111,6 +121,9 @@
   <si>
     <t>left_prosocial</t>
   </si>
+  <si>
+    <t>rule_J</t>
+  </si>
 </sst>
 </file>
 
@@ -159,17 +172,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7814,19 +7817,14 @@
       <sortCondition ref="N1:N81"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",Z1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:W81">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+  <conditionalFormatting sqref="R2:W81">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:U81">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="Z1:Z1048576">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",Z1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7849,7 +7847,7 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B32" ca="1" si="0">RANDBETWEEN(1,10000)</f>
-        <v>2143</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -7858,7 +7856,7 @@
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>2328</v>
+        <v>9320</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -7867,7 +7865,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>1128</v>
+        <v>6363</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -7876,7 +7874,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>2918</v>
+        <v>7571</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -7885,7 +7883,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>4307</v>
+        <v>8126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -7894,7 +7892,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>2477</v>
+        <v>8281</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -7903,7 +7901,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>7193</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -7912,7 +7910,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>7204</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -7921,7 +7919,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1684</v>
+        <v>8766</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -7930,7 +7928,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>1428</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -7939,7 +7937,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>1687</v>
+        <v>8213</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -7948,7 +7946,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5768</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -7957,7 +7955,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6748</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -7966,7 +7964,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>4474</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -7975,7 +7973,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7842</v>
+        <v>4927</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -7984,7 +7982,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>2384</v>
+        <v>8508</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -7993,7 +7991,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>855</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -8002,7 +8000,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>9503</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -8011,7 +8009,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>988</v>
+        <v>9761</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -8020,7 +8018,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>4774</v>
+        <v>5267</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -8029,7 +8027,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>5803</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -8038,7 +8036,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>4302</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -8047,7 +8045,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>487</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -8056,7 +8054,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>9177</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -8065,7 +8063,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>8192</v>
+        <v>9225</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -8074,7 +8072,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>4032</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -8083,7 +8081,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>3699</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -8092,7 +8090,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>2894</v>
+        <v>5916</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -8101,7 +8099,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>3401</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -8110,7 +8108,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>591</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -8119,7 +8117,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>3360</v>
+        <v>8182</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -8128,7 +8126,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>7886</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -8137,7 +8135,7 @@
       </c>
       <c r="B33">
         <f t="shared" ref="B33:B64" ca="1" si="1">RANDBETWEEN(1,10000)</f>
-        <v>9134</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -8146,7 +8144,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>226</v>
+        <v>9688</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -8155,7 +8153,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>1901</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -8164,7 +8162,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>3722</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -8173,7 +8171,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>7828</v>
+        <v>8065</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -8182,7 +8180,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>3834</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -8191,7 +8189,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>8436</v>
+        <v>5968</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -8200,7 +8198,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>5591</v>
+        <v>5814</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -8209,7 +8207,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>9688</v>
+        <v>9991</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -8218,7 +8216,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>1042</v>
+        <v>6945</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -8227,7 +8225,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>9380</v>
+        <v>9956</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -8236,7 +8234,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>5248</v>
+        <v>8994</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -8245,7 +8243,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>5937</v>
+        <v>7379</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -8254,7 +8252,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>9662</v>
+        <v>577</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -8263,7 +8261,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>8460</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -8272,7 +8270,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>4576</v>
+        <v>9103</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -8281,7 +8279,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>9352</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -8290,7 +8288,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>5190</v>
+        <v>566</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -8299,7 +8297,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>2037</v>
+        <v>7999</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -8308,7 +8306,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>3916</v>
+        <v>8975</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -8317,7 +8315,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>6112</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -8326,7 +8324,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>5406</v>
+        <v>7716</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -8335,7 +8333,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>3975</v>
+        <v>8237</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -8344,7 +8342,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>336</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -8353,7 +8351,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>2675</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -8362,7 +8360,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>4012</v>
+        <v>8583</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -8371,7 +8369,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>8188</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -8380,7 +8378,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>737</v>
+        <v>8495</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -8389,7 +8387,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>1091</v>
+        <v>9590</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -8398,7 +8396,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>612</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -8407,7 +8405,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>7915</v>
+        <v>823</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -8416,7 +8414,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>7772</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -8425,7 +8423,7 @@
       </c>
       <c r="B65">
         <f t="shared" ref="B65:B80" ca="1" si="2">RANDBETWEEN(1,10000)</f>
-        <v>3444</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -8434,7 +8432,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="2"/>
-        <v>8117</v>
+        <v>8309</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -8443,7 +8441,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="2"/>
-        <v>6913</v>
+        <v>5660</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -8452,7 +8450,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="2"/>
-        <v>5599</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -8461,7 +8459,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="2"/>
-        <v>2107</v>
+        <v>5115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -8470,7 +8468,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="2"/>
-        <v>5803</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -8479,7 +8477,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>1122</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -8488,7 +8486,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="2"/>
-        <v>7008</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -8497,7 +8495,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="2"/>
-        <v>6116</v>
+        <v>6688</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -8506,7 +8504,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="2"/>
-        <v>4514</v>
+        <v>684</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -8515,7 +8513,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="2"/>
-        <v>296</v>
+        <v>5338</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -8524,7 +8522,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="2"/>
-        <v>9359</v>
+        <v>2838</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -8533,7 +8531,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>6376</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -8542,7 +8540,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="2"/>
-        <v>8956</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -8551,7 +8549,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="2"/>
-        <v>2046</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -8560,7 +8558,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="2"/>
-        <v>5966</v>
+        <v>8361</v>
       </c>
     </row>
   </sheetData>
@@ -8578,7 +8576,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8633,7 +8631,7 @@
         <v>9</v>
       </c>
       <c r="Q1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
@@ -12065,14 +12063,14 @@
       <sortCondition ref="O1:O65"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="O1:O61">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",O1)))</formula>
+  <conditionalFormatting sqref="G2:L61">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:L61">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="O1:O61">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>